<commit_message>
Added Commands: B, IM, I, i
</commit_message>
<xml_diff>
--- a/frva/src/main/java/controller/util/liveviewparser/_RoxCommands.xlsx
+++ b/frva/src/main/java/controller/util/liveviewparser/_RoxCommands.xlsx
@@ -193,7 +193,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,13 +209,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -227,14 +251,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -558,7 +588,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,13 +629,16 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -648,13 +681,16 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E8" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -670,38 +706,46 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F10" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E11" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F12" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -750,32 +794,42 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E17" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E18" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F19" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>